<commit_message>
EPL Coaches w/xValues; first version of betting matrix
</commit_message>
<xml_diff>
--- a/Coaches_carreers/Coaches/Daniel Farke.xlsx
+++ b/Coaches_carreers/Coaches/Daniel Farke.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE131"/>
+  <dimension ref="A1:AF131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,6 +593,11 @@
           <t>ProbA</t>
         </is>
       </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -698,6 +703,11 @@
       <c r="AE2" t="n">
         <v>0.259620596205962</v>
       </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -803,6 +813,11 @@
       <c r="AE3" t="n">
         <v>0.2124124124124125</v>
       </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -908,6 +923,11 @@
       <c r="AE4" t="n">
         <v>0.2135820030556873</v>
       </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1013,6 +1033,11 @@
       <c r="AE5" t="n">
         <v>0.3047385620915032</v>
       </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1118,6 +1143,11 @@
       <c r="AE6" t="n">
         <v>0.3615520282186949</v>
       </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1223,6 +1253,11 @@
       <c r="AE7" t="n">
         <v>0.2135820030556873</v>
       </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1328,6 +1363,11 @@
       <c r="AE8" t="n">
         <v>0.1095669036845508</v>
       </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1433,6 +1473,11 @@
       <c r="AE9" t="n">
         <v>0.3346469622331691</v>
       </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1538,6 +1583,11 @@
       <c r="AE10" t="n">
         <v>0.241340530814215</v>
       </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1643,6 +1693,11 @@
       <c r="AE11" t="n">
         <v>0.2285307285307285</v>
       </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1748,6 +1803,11 @@
       <c r="AE12" t="n">
         <v>0.3619907764394456</v>
       </c>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1852,6 +1912,11 @@
       </c>
       <c r="AE13" t="n">
         <v>0.2532163742690059</v>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -1958,6 +2023,11 @@
       <c r="AE14" t="n">
         <v>0.445442626858556</v>
       </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2063,6 +2133,11 @@
       <c r="AE15" t="n">
         <v>0.257019454323234</v>
       </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2168,6 +2243,11 @@
       <c r="AE16" t="n">
         <v>0.3624441836450591</v>
       </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2273,6 +2353,11 @@
       <c r="AE17" t="n">
         <v>0.4693121693121693</v>
       </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2378,6 +2463,11 @@
       <c r="AE18" t="n">
         <v>0.1928571428571429</v>
       </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2483,6 +2573,11 @@
       <c r="AE19" t="n">
         <v>0.3484557709856161</v>
       </c>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2588,6 +2683,11 @@
       <c r="AE20" t="n">
         <v>0.2621907621907622</v>
       </c>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2693,6 +2793,11 @@
       <c r="AE21" t="n">
         <v>0.2460761511116872</v>
       </c>
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2798,6 +2903,11 @@
       <c r="AE22" t="n">
         <v>0.2994861454590367</v>
       </c>
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2903,6 +3013,11 @@
       <c r="AE23" t="n">
         <v>0.277332958748888</v>
       </c>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3008,6 +3123,11 @@
       <c r="AE24" t="n">
         <v>0.3139378003161635</v>
       </c>
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3113,6 +3233,11 @@
       <c r="AE25" t="n">
         <v>0.4097782776481818</v>
       </c>
+      <c r="AF25" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3218,6 +3343,11 @@
       <c r="AE26" t="n">
         <v>0.4691319005478298</v>
       </c>
+      <c r="AF26" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3323,6 +3453,11 @@
       <c r="AE27" t="n">
         <v>0.2675171834050339</v>
       </c>
+      <c r="AF27" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3428,6 +3563,11 @@
       <c r="AE28" t="n">
         <v>0.2861013426766799</v>
       </c>
+      <c r="AF28" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3533,6 +3673,11 @@
       <c r="AE29" t="n">
         <v>0.349752715572894</v>
       </c>
+      <c r="AF29" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3638,6 +3783,11 @@
       <c r="AE30" t="n">
         <v>0.2401709401709401</v>
       </c>
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3743,6 +3893,11 @@
       <c r="AE31" t="n">
         <v>0.353719160170773</v>
       </c>
+      <c r="AF31" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3848,6 +4003,11 @@
       <c r="AE32" t="n">
         <v>0.245148315736551</v>
       </c>
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3953,6 +4113,11 @@
       <c r="AE33" t="n">
         <v>0.1594771241830065</v>
       </c>
+      <c r="AF33" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4058,6 +4223,11 @@
       <c r="AE34" t="n">
         <v>0.1345482923246419</v>
       </c>
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4163,6 +4333,11 @@
       <c r="AE35" t="n">
         <v>0.1455247650899825</v>
       </c>
+      <c r="AF35" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4268,6 +4443,11 @@
       <c r="AE36" t="n">
         <v>0.1912483912483913</v>
       </c>
+      <c r="AF36" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4373,6 +4553,11 @@
       <c r="AE37" t="n">
         <v>0.3390878253818034</v>
       </c>
+      <c r="AF37" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4478,6 +4663,11 @@
       <c r="AE38" t="n">
         <v>0.3549661401411573</v>
       </c>
+      <c r="AF38" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4583,6 +4773,11 @@
       <c r="AE39" t="n">
         <v>0.200911437753543</v>
       </c>
+      <c r="AF39" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4688,6 +4883,11 @@
       <c r="AE40" t="n">
         <v>0.445442626858556</v>
       </c>
+      <c r="AF40" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4793,6 +4993,11 @@
       <c r="AE41" t="n">
         <v>0.3238938053097345</v>
       </c>
+      <c r="AF41" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4898,6 +5103,11 @@
       <c r="AE42" t="n">
         <v>0.3760683760683761</v>
       </c>
+      <c r="AF42" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5003,6 +5213,11 @@
       <c r="AE43" t="n">
         <v>0.3730738512811894</v>
       </c>
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5108,6 +5323,11 @@
       <c r="AE44" t="n">
         <v>0.3995868782378305</v>
       </c>
+      <c r="AF44" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5213,6 +5433,11 @@
       <c r="AE45" t="n">
         <v>0.1808292077916039</v>
       </c>
+      <c r="AF45" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5318,6 +5543,11 @@
       <c r="AE46" t="n">
         <v>0.2133505537199468</v>
       </c>
+      <c r="AF46" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5423,6 +5653,11 @@
       <c r="AE47" t="n">
         <v>0.3739815457372709</v>
       </c>
+      <c r="AF47" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5528,6 +5763,11 @@
       <c r="AE48" t="n">
         <v>0.3263403263403264</v>
       </c>
+      <c r="AF48" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -5633,6 +5873,11 @@
       <c r="AE49" t="n">
         <v>0.3492063492063492</v>
       </c>
+      <c r="AF49" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -5738,6 +5983,11 @@
       <c r="AE50" t="n">
         <v>0.2571428571428572</v>
       </c>
+      <c r="AF50" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -5843,6 +6093,11 @@
       <c r="AE51" t="n">
         <v>0.3047385620915032</v>
       </c>
+      <c r="AF51" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -5948,6 +6203,11 @@
       <c r="AE52" t="n">
         <v>0.3609955766818512</v>
       </c>
+      <c r="AF52" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -6053,6 +6313,11 @@
       <c r="AE53" t="n">
         <v>0.3760683760683761</v>
       </c>
+      <c r="AF53" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -6158,6 +6423,11 @@
       <c r="AE54" t="n">
         <v>0.3857095406498505</v>
       </c>
+      <c r="AF54" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -6263,6 +6533,11 @@
       <c r="AE55" t="n">
         <v>0.3776223776223777</v>
       </c>
+      <c r="AF55" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -6368,6 +6643,11 @@
       <c r="AE56" t="n">
         <v>0.3241830065359477</v>
       </c>
+      <c r="AF56" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -6473,6 +6753,11 @@
       <c r="AE57" t="n">
         <v>0.2864450127877238</v>
       </c>
+      <c r="AF57" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -6578,6 +6863,11 @@
       <c r="AE58" t="n">
         <v>0.2549694742628975</v>
       </c>
+      <c r="AF58" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -6683,6 +6973,11 @@
       <c r="AE59" t="n">
         <v>0.3140436624307592</v>
       </c>
+      <c r="AF59" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -6788,6 +7083,11 @@
       <c r="AE60" t="n">
         <v>0.3047385620915032</v>
       </c>
+      <c r="AF60" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -6893,6 +7193,11 @@
       <c r="AE61" t="n">
         <v>0.2864450127877238</v>
       </c>
+      <c r="AF61" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -6998,6 +7303,11 @@
       <c r="AE62" t="n">
         <v>0.3125020254460842</v>
       </c>
+      <c r="AF62" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -7103,6 +7413,11 @@
       <c r="AE63" t="n">
         <v>0.4269402095489052</v>
       </c>
+      <c r="AF63" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -7208,6 +7523,11 @@
       <c r="AE64" t="n">
         <v>0.2124124124124125</v>
       </c>
+      <c r="AF64" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -7313,6 +7633,11 @@
       <c r="AE65" t="n">
         <v>0.3241830065359477</v>
       </c>
+      <c r="AF65" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -7418,6 +7743,11 @@
       <c r="AE66" t="n">
         <v>0.4570291252534243</v>
       </c>
+      <c r="AF66" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -7523,6 +7853,11 @@
       <c r="AE67" t="n">
         <v>0.1062091503267974</v>
       </c>
+      <c r="AF67" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -7628,6 +7963,11 @@
       <c r="AE68" t="n">
         <v>0.08217468805704102</v>
       </c>
+      <c r="AF68" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -7733,6 +8073,11 @@
       <c r="AE69" t="n">
         <v>0.3718336297962515</v>
       </c>
+      <c r="AF69" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -7838,6 +8183,11 @@
       <c r="AE70" t="n">
         <v>0.3998760794640436</v>
       </c>
+      <c r="AF70" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -7943,6 +8293,11 @@
       <c r="AE71" t="n">
         <v>0.2217692348967419</v>
       </c>
+      <c r="AF71" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -8048,6 +8403,11 @@
       <c r="AE72" t="n">
         <v>0.2726423902894491</v>
       </c>
+      <c r="AF72" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -8153,6 +8513,11 @@
       <c r="AE73" t="n">
         <v>0.3367466997659776</v>
       </c>
+      <c r="AF73" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -8258,6 +8623,11 @@
       <c r="AE74" t="n">
         <v>0.2946127946127946</v>
       </c>
+      <c r="AF74" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -8363,6 +8733,11 @@
       <c r="AE75" t="n">
         <v>0.2168172957646642</v>
       </c>
+      <c r="AF75" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -8468,6 +8843,11 @@
       <c r="AE76" t="n">
         <v>0.3241830065359477</v>
       </c>
+      <c r="AF76" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -8573,6 +8953,11 @@
       <c r="AE77" t="n">
         <v>0.241340530814215</v>
       </c>
+      <c r="AF77" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -8678,6 +9063,11 @@
       <c r="AE78" t="n">
         <v>0.1026455026455026</v>
       </c>
+      <c r="AF78" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -8783,6 +9173,11 @@
       <c r="AE79" t="n">
         <v>0.347985347985348</v>
       </c>
+      <c r="AF79" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -8888,6 +9283,11 @@
       <c r="AE80" t="n">
         <v>0.5815508021390374</v>
       </c>
+      <c r="AF80" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -8993,6 +9393,11 @@
       <c r="AE81" t="n">
         <v>0.2401709401709401</v>
       </c>
+      <c r="AF81" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -9098,6 +9503,11 @@
       <c r="AE82" t="n">
         <v>0.4457318280847692</v>
       </c>
+      <c r="AF82" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -9203,6 +9613,11 @@
       <c r="AE83" t="n">
         <v>0.1801491681009753</v>
       </c>
+      <c r="AF83" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -9308,6 +9723,11 @@
       <c r="AE84" t="n">
         <v>0.1639597349131439</v>
       </c>
+      <c r="AF84" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -9413,6 +9833,11 @@
       <c r="AE85" t="n">
         <v>0.5974025974025974</v>
       </c>
+      <c r="AF85" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -9518,6 +9943,11 @@
       <c r="AE86" t="n">
         <v>0.3826500297088533</v>
       </c>
+      <c r="AF86" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -9623,6 +10053,11 @@
       <c r="AE87" t="n">
         <v>0.115009746588694</v>
       </c>
+      <c r="AF87" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -9728,6 +10163,11 @@
       <c r="AE88" t="n">
         <v>0.1017033075856605</v>
       </c>
+      <c r="AF88" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -9833,6 +10273,11 @@
       <c r="AE89" t="n">
         <v>0.547356330266261</v>
       </c>
+      <c r="AF89" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -9938,6 +10383,11 @@
       <c r="AE90" t="n">
         <v>0.1349489290665761</v>
       </c>
+      <c r="AF90" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -10043,6 +10493,11 @@
       <c r="AE91" t="n">
         <v>0.4799651567944251</v>
       </c>
+      <c r="AF91" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -10148,6 +10603,11 @@
       <c r="AE92" t="n">
         <v>0.1104575163398693</v>
       </c>
+      <c r="AF92" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -10253,6 +10713,11 @@
       <c r="AE93" t="n">
         <v>0.3924648786717752</v>
       </c>
+      <c r="AF93" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -10358,6 +10823,11 @@
       <c r="AE94" t="n">
         <v>0.04269005847953213</v>
       </c>
+      <c r="AF94" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -10463,6 +10933,11 @@
       <c r="AE95" t="n">
         <v>0.2861952861952862</v>
       </c>
+      <c r="AF95" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -10568,6 +11043,11 @@
       <c r="AE96" t="n">
         <v>0.5378325207424515</v>
       </c>
+      <c r="AF96" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -10673,6 +11153,11 @@
       <c r="AE97" t="n">
         <v>0.2386232386232387</v>
       </c>
+      <c r="AF97" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -10778,6 +11263,11 @@
       <c r="AE98" t="n">
         <v>0.858869395711501</v>
       </c>
+      <c r="AF98" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -10882,6 +11372,11 @@
       </c>
       <c r="AE99" t="n">
         <v>0.2694235588972432</v>
+      </c>
+      <c r="AF99" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
       </c>
     </row>
     <row r="100">
@@ -10988,6 +11483,11 @@
       <c r="AE100" t="n">
         <v>0.2467836257309942</v>
       </c>
+      <c r="AF100" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -11093,6 +11593,11 @@
       <c r="AE101" t="n">
         <v>0.3381890027459648</v>
       </c>
+      <c r="AF101" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -11198,6 +11703,11 @@
       <c r="AE102" t="n">
         <v>0.2188999630860096</v>
       </c>
+      <c r="AF102" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -11303,6 +11813,11 @@
       <c r="AE103" t="n">
         <v>0.5539700868800176</v>
       </c>
+      <c r="AF103" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -11408,6 +11923,11 @@
       <c r="AE104" t="n">
         <v>0.2141343925005776</v>
       </c>
+      <c r="AF104" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -11513,6 +12033,11 @@
       <c r="AE105" t="n">
         <v>0.3760763564685133</v>
       </c>
+      <c r="AF105" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -11618,6 +12143,11 @@
       <c r="AE106" t="n">
         <v>0.1062091503267974</v>
       </c>
+      <c r="AF106" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -11723,6 +12253,11 @@
       <c r="AE107" t="n">
         <v>0.5539700868800176</v>
       </c>
+      <c r="AF107" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -11828,6 +12363,11 @@
       <c r="AE108" t="n">
         <v>0.2149317091177556</v>
       </c>
+      <c r="AF108" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -11933,6 +12473,11 @@
       <c r="AE109" t="n">
         <v>0.404446661539634</v>
       </c>
+      <c r="AF109" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -12038,6 +12583,11 @@
       <c r="AE110" t="n">
         <v>0.06010928961748631</v>
       </c>
+      <c r="AF110" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -12143,6 +12693,11 @@
       <c r="AE111" t="n">
         <v>0.5076023391812865</v>
       </c>
+      <c r="AF111" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -12248,6 +12803,11 @@
       <c r="AE112" t="n">
         <v>0.2877344877344877</v>
       </c>
+      <c r="AF112" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -12353,6 +12913,11 @@
       <c r="AE113" t="n">
         <v>0.5849397590361446</v>
       </c>
+      <c r="AF113" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -12458,6 +13023,11 @@
       <c r="AE114" t="n">
         <v>0.3443850267379679</v>
       </c>
+      <c r="AF114" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -12563,6 +13133,11 @@
       <c r="AE115" t="n">
         <v>0.09764607597424936</v>
       </c>
+      <c r="AF115" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -12668,6 +13243,11 @@
       <c r="AE116" t="n">
         <v>0.2917082917082918</v>
       </c>
+      <c r="AF116" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -12773,6 +13353,11 @@
       <c r="AE117" t="n">
         <v>0.1174603174603174</v>
       </c>
+      <c r="AF117" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -12878,6 +13463,11 @@
       <c r="AE118" t="n">
         <v>0.2857991681521093</v>
       </c>
+      <c r="AF118" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -12983,6 +13573,11 @@
       <c r="AE119" t="n">
         <v>0.7830303030303031</v>
       </c>
+      <c r="AF119" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -13088,6 +13683,11 @@
       <c r="AE120" t="n">
         <v>0.126984126984127</v>
       </c>
+      <c r="AF120" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -13193,6 +13793,11 @@
       <c r="AE121" t="n">
         <v>0.5626471254776462</v>
       </c>
+      <c r="AF121" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -13298,6 +13903,11 @@
       <c r="AE122" t="n">
         <v>0.1583662714097496</v>
       </c>
+      <c r="AF122" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -13403,6 +14013,11 @@
       <c r="AE123" t="n">
         <v>0.391156462585034</v>
       </c>
+      <c r="AF123" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -13508,6 +14123,11 @@
       <c r="AE124" t="n">
         <v>0.5061478482531113</v>
       </c>
+      <c r="AF124" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -13613,6 +14233,11 @@
       <c r="AE125" t="n">
         <v>0.1269145084934559</v>
       </c>
+      <c r="AF125" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -13718,6 +14343,11 @@
       <c r="AE126" t="n">
         <v>0.4373143196672608</v>
       </c>
+      <c r="AF126" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -13823,6 +14453,11 @@
       <c r="AE127" t="n">
         <v>0.1816993464052288</v>
       </c>
+      <c r="AF127" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -13928,6 +14563,11 @@
       <c r="AE128" t="n">
         <v>0.4974358974358975</v>
       </c>
+      <c r="AF128" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -14033,6 +14673,11 @@
       <c r="AE129" t="n">
         <v>0.03984225269054996</v>
       </c>
+      <c r="AF129" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -14138,6 +14783,11 @@
       <c r="AE130" t="n">
         <v>0.4274237472766884</v>
       </c>
+      <c r="AF130" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -14242,6 +14892,11 @@
       </c>
       <c r="AE131" t="n">
         <v>0.02002935336268673</v>
+      </c>
+      <c r="AF131" t="inlineStr">
+        <is>
+          <t>Norwich</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>